<commit_message>
first draft of weigo report results
</commit_message>
<xml_diff>
--- a/Tables/SS.xlsx
+++ b/Tables/SS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Statistics\P27\IMSS\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAECEEAB-7CCF-4C3A-BE0D-9D30EBC2FB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7561B1D-7910-43B7-BE54-ADD1716C3006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15510" yWindow="-4785" windowWidth="14400" windowHeight="8175" xr2:uid="{DDC5E293-EDB8-4005-A2FB-235A67631FB3}"/>
+    <workbookView xWindow="-18570" yWindow="-6120" windowWidth="13245" windowHeight="11760" xr2:uid="{DDC5E293-EDB8-4005-A2FB-235A67631FB3}"/>
   </bookViews>
   <sheets>
     <sheet name="SS_0" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>No IMSS</t>
   </si>
@@ -46,13 +46,7 @@
     <t>No SAT</t>
   </si>
   <si>
-    <t>[2000-2004]</t>
-  </si>
-  <si>
     <t>[2005-2010]</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Informal INEGI</t>
@@ -195,82 +189,61 @@
           <cell r="E1" t="str">
             <v>(2)</v>
           </cell>
-          <cell r="G1" t="str">
-            <v>(3)</v>
-          </cell>
         </row>
         <row r="4">
+          <cell r="B4" t="str">
+            <v>1.08e+09</v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>0.595</v>
+          </cell>
           <cell r="D4" t="str">
-            <v>1.08e+09</v>
+            <v>991520597</v>
           </cell>
           <cell r="E4" t="str">
-            <v>0.595</v>
-          </cell>
-          <cell r="F4" t="str">
-            <v>991520597</v>
-          </cell>
-          <cell r="G4" t="str">
             <v>0.591</v>
           </cell>
         </row>
         <row r="5">
           <cell r="D5">
-            <v>4080591</v>
-          </cell>
-          <cell r="F5">
             <v>3359681</v>
           </cell>
         </row>
         <row r="6">
           <cell r="B6" t="str">
-            <v>256907371</v>
+            <v>1.08e+09</v>
           </cell>
           <cell r="C6" t="str">
-            <v>0.220</v>
+            <v>0.730</v>
           </cell>
           <cell r="D6" t="str">
-            <v>1.08e+09</v>
+            <v>986199081</v>
           </cell>
           <cell r="E6" t="str">
-            <v>0.730</v>
-          </cell>
-          <cell r="F6" t="str">
-            <v>986199081</v>
-          </cell>
-          <cell r="G6" t="str">
             <v>0.718</v>
           </cell>
         </row>
         <row r="7">
-          <cell r="B7">
-            <v>1705253</v>
-          </cell>
           <cell r="D7">
-            <v>4058685</v>
-          </cell>
-          <cell r="F7">
             <v>3342419</v>
           </cell>
         </row>
         <row r="8">
+          <cell r="B8" t="str">
+            <v>447076824</v>
+          </cell>
+          <cell r="C8" t="str">
+            <v>0.972</v>
+          </cell>
           <cell r="D8" t="str">
-            <v>447076824</v>
+            <v>406802632</v>
           </cell>
           <cell r="E8" t="str">
-            <v>0.972</v>
-          </cell>
-          <cell r="F8" t="str">
-            <v>406802632</v>
-          </cell>
-          <cell r="G8" t="str">
             <v>0.953</v>
           </cell>
         </row>
         <row r="9">
           <cell r="D9">
-            <v>1669329</v>
-          </cell>
-          <cell r="F9">
             <v>1368900</v>
           </cell>
         </row>
@@ -577,38 +550,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{492B3CD1-942B-479B-A390-BFEEB7BE96F5}">
-  <dimension ref="A4:G18"/>
+  <dimension ref="A4:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="6"/>
       <c r="B4" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="str">
         <f>[1]Sheet1!A1</f>
         <v/>
@@ -621,164 +590,130 @@
         <f>[1]Sheet1!E1</f>
         <v>(2)</v>
       </c>
-      <c r="D6" s="5" t="str">
-        <f>[1]Sheet1!G1</f>
-        <v>(3)</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <f>[1]Sheet1!C4</f>
+        <v>0.595</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>[1]Sheet1!E4</f>
-        <v>0.595</v>
-      </c>
-      <c r="D7" s="1" t="str">
-        <f>[1]Sheet1!G4</f>
         <v>0.591</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <f>[1]Sheet1!$D$5</f>
+        <v>3359681</v>
       </c>
       <c r="C8" s="1">
         <f>[1]Sheet1!$D$5</f>
-        <v>4080591</v>
-      </c>
-      <c r="D8" s="1">
-        <f>[1]Sheet1!$F$5</f>
         <v>3359681</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <f>[1]Sheet1!B4</f>
+        <v>1.08e+09</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>[1]Sheet1!D4</f>
-        <v>1.08e+09</v>
-      </c>
-      <c r="D9" s="1" t="str">
-        <f>[1]Sheet1!F4</f>
         <v>991520597</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="1" t="str">
         <f>[1]Sheet1!C6</f>
-        <v>0.220</v>
+        <v>0.730</v>
       </c>
       <c r="C11" s="1" t="str">
         <f>[1]Sheet1!E6</f>
-        <v>0.730</v>
-      </c>
-      <c r="D11" s="1" t="str">
-        <f>[1]Sheet1!G6</f>
         <v>0.718</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1">
-        <f>[1]Sheet1!$B$7</f>
-        <v>1705253</v>
+        <f>[1]Sheet1!$D$7</f>
+        <v>3342419</v>
       </c>
       <c r="C12" s="1">
         <f>[1]Sheet1!$D$7</f>
-        <v>4058685</v>
-      </c>
-      <c r="D12" s="1">
-        <f>[1]Sheet1!$F$7</f>
         <v>3342419</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1" t="str">
         <f>[1]Sheet1!B6</f>
-        <v>256907371</v>
+        <v>1.08e+09</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>[1]Sheet1!D6</f>
-        <v>1.08e+09</v>
-      </c>
-      <c r="D13" s="1" t="str">
-        <f>[1]Sheet1!F6</f>
         <v>986199081</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>4</v>
+      <c r="B15" s="1" t="str">
+        <f>[1]Sheet1!C8</f>
+        <v>0.972</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>[1]Sheet1!E8</f>
-        <v>0.972</v>
-      </c>
-      <c r="D15" s="1" t="str">
-        <f>[1]Sheet1!G8</f>
         <v>0.953</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B16" s="1">
+        <f>[1]Sheet1!$D$9</f>
+        <v>1368900</v>
       </c>
       <c r="C16" s="1">
         <f>[1]Sheet1!$D$9</f>
-        <v>1669329</v>
-      </c>
-      <c r="D16" s="1">
-        <f>[1]Sheet1!$F$9</f>
         <v>1368900</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="B17" s="3" t="str">
+        <f>[1]Sheet1!B8</f>
+        <v>447076824</v>
       </c>
       <c r="C17" s="3" t="str">
         <f>[1]Sheet1!D8</f>
-        <v>447076824</v>
-      </c>
-      <c r="D17" s="3" t="str">
-        <f>[1]Sheet1!F8</f>
         <v>406802632</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>